<commit_message>
about page in usdt
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_usdt.xlsx
+++ b/tests/frameworks/framework_usdt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/frameworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE52563-4681-47D5-A8A4-0EF1BD0DBBFC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C752EAB5-16C6-D64C-AA3F-D82C60203996}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Parameters" sheetId="6" r:id="rId6"/>
     <sheet name="Cascades" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -938,7 +938,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>Code Name</t>
   </si>
@@ -1123,9 +1123,6 @@
     <t>USDT</t>
   </si>
   <si>
-    <t>USDT cascade</t>
-  </si>
-  <si>
     <t>Targetable</t>
   </si>
   <si>
@@ -1139,6 +1136,54 @@
   </si>
   <si>
     <t>num_loss/max(tx,num_loss)</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Use this file to specify the structure of your model. Any extra sheets will be ignored, so you can include other information in them</t>
+  </si>
+  <si>
+    <t>Page Overview</t>
+  </si>
+  <si>
+    <t>Databook Pages</t>
+  </si>
+  <si>
+    <t>Specify which worksheets will be present in the databook</t>
+  </si>
+  <si>
+    <t>Compartments</t>
+  </si>
+  <si>
+    <t>Specify the states that an individual can be in - an individual is only ever in one compartment at a time</t>
+  </si>
+  <si>
+    <t>Transitions</t>
+  </si>
+  <si>
+    <t>Specify which transitions between compartments are possible</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>Specify groups of people (e.g. groups of compartments) for data entry</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Define how to compute the flows between compartments</t>
+  </si>
+  <si>
+    <t>Cascades</t>
+  </si>
+  <si>
+    <t>Use the Cascades sheet to define the cascade if it is more complex than just all characteristics in sequence</t>
+  </si>
+  <si>
+    <t>Framework for a 4-stage cascade model, without vital dynamics or new cases</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1191,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1203,7 +1248,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1220,7 +1265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1568,15 +1613,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77F58F0-B063-4640-9F39-D0203701916E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="97.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
@@ -1584,12 +1633,75 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>61</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1605,13 +1717,13 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1619,7 +1731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1627,39 +1739,39 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
@@ -1677,17 +1789,17 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1819,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1725,7 +1837,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -1743,7 +1855,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1761,7 +1873,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -1798,9 +1910,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="str">
         <f>Compartments!$A$2</f>
         <v>undx</v>
@@ -1818,7 +1930,7 @@
         <v>tx</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>Compartments!$A$2</f>
         <v>undx</v>
@@ -1827,7 +1939,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>Compartments!$A$3</f>
         <v>scr</v>
@@ -1836,7 +1948,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>Compartments!$A$4</f>
         <v>dx</v>
@@ -1845,7 +1957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f>Compartments!$A$5</f>
         <v>tx</v>
@@ -1867,16 +1979,16 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1893,7 +2005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -1910,7 +2022,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -1927,7 +2039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -1944,7 +2056,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1971,24 +2083,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="111" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2011,13 +2123,13 @@
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -2040,7 +2152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>50</v>
       </c>
@@ -2058,14 +2170,14 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -2088,7 +2200,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -2106,14 +2218,14 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
@@ -2136,7 +2248,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2154,14 +2266,14 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -2184,7 +2296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2202,14 +2314,14 @@
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="7"/>
       <c r="C10" s="2"/>
@@ -2220,7 +2332,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2230,7 +2342,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2240,7 +2352,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2250,7 +2362,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2260,7 +2372,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2270,7 +2382,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2280,7 +2392,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2290,7 +2402,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2300,7 +2412,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2310,7 +2422,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2320,7 +2432,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2353,13 +2465,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2367,7 +2479,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -2375,7 +2487,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -2383,7 +2495,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -2391,7 +2503,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>

</xml_diff>